<commit_message>
My Portion of the SQL File
</commit_message>
<xml_diff>
--- a/DWBuildTracking.xlsx
+++ b/DWBuildTracking.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t>Deliverable</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Raleigh</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -427,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B18"/>
+  <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,31 +446,40 @@
     <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -472,55 +487,71 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -528,7 +559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
@@ -536,7 +567,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -544,7 +575,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -552,7 +583,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>